<commit_message>
Agregar aplicaciÃ³n Streamlit y refactorizaciÃ³n de mÃ³dulos
- Nueva aplicaciÃ³n Streamlit con interfaz de 3 pestaÃ±as
- RefactorizaciÃ³n de cÃ³digo en mÃ³dulos utils/ (helpers, data_loader, data_processor, cluster_processor, processor)
- CorrecciÃ³n de error con Duraznos Blancos (clustering con valores duplicados)
- DocumentaciÃ³n completa del proyecto (README.txt, anÃ¡lisis, instrucciones)
- ActualizaciÃ³n de requirements.txt con streamlit
- CreaciÃ³n de .gitignore para excluir env/ y archivos temporales
</commit_message>
<xml_diff>
--- a/Data/Lotes_DuraznoBl.xlsx
+++ b/Data/Lotes_DuraznoBl.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorja\Desktop\CarozosTodo\Carozosgpt\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorja\Desktop\Carozosapp\Carozosapp\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDDA0CE-C848-4C92-9E38-E3402E71791C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8E7DDC-6A53-4A62-AC12-6FC12D78C8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{5564C5AD-00E3-4865-BD95-E148CF4E0047}"/>
   </bookViews>
@@ -227,9 +227,6 @@
     <t>AGRICOLA EL CANELO LIMITADA</t>
   </si>
   <si>
-    <t>LINEA PRODUCTOS</t>
-  </si>
-  <si>
     <t>ESPECIE</t>
   </si>
   <si>
@@ -237,6 +234,9 @@
   </si>
   <si>
     <t>BLANCOS</t>
+  </si>
+  <si>
+    <t>LINEA PRODUCTO</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83981A1E-71E4-49ED-9969-4826C51039C6}">
   <dimension ref="A1:BE83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -619,10 +621,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -792,10 +794,10 @@
         <v>115</v>
       </c>
       <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
         <v>65</v>
-      </c>
-      <c r="C2" t="s">
-        <v>66</v>
       </c>
       <c r="D2" t="s">
         <v>58</v>
@@ -965,10 +967,10 @@
         <v>116</v>
       </c>
       <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
         <v>65</v>
-      </c>
-      <c r="C3" t="s">
-        <v>66</v>
       </c>
       <c r="D3" t="s">
         <v>59</v>
@@ -1138,10 +1140,10 @@
         <v>117</v>
       </c>
       <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
         <v>65</v>
-      </c>
-      <c r="C4" t="s">
-        <v>66</v>
       </c>
       <c r="D4" t="s">
         <v>58</v>
@@ -1311,10 +1313,10 @@
         <v>118</v>
       </c>
       <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
         <v>65</v>
-      </c>
-      <c r="C5" t="s">
-        <v>66</v>
       </c>
       <c r="D5" t="s">
         <v>59</v>
@@ -1484,10 +1486,10 @@
         <v>119</v>
       </c>
       <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
         <v>65</v>
-      </c>
-      <c r="C6" t="s">
-        <v>66</v>
       </c>
       <c r="D6" t="s">
         <v>58</v>
@@ -1657,10 +1659,10 @@
         <v>120</v>
       </c>
       <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
         <v>65</v>
-      </c>
-      <c r="C7" t="s">
-        <v>66</v>
       </c>
       <c r="D7" t="s">
         <v>59</v>
@@ -1830,10 +1832,10 @@
         <v>121</v>
       </c>
       <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
         <v>65</v>
-      </c>
-      <c r="C8" t="s">
-        <v>66</v>
       </c>
       <c r="D8" t="s">
         <v>60</v>
@@ -2003,10 +2005,10 @@
         <v>122</v>
       </c>
       <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
         <v>65</v>
-      </c>
-      <c r="C9" t="s">
-        <v>66</v>
       </c>
       <c r="D9" t="s">
         <v>58</v>
@@ -2176,10 +2178,10 @@
         <v>123</v>
       </c>
       <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
         <v>65</v>
-      </c>
-      <c r="C10" t="s">
-        <v>66</v>
       </c>
       <c r="D10" t="s">
         <v>60</v>
@@ -2349,10 +2351,10 @@
         <v>124</v>
       </c>
       <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
         <v>65</v>
-      </c>
-      <c r="C11" t="s">
-        <v>66</v>
       </c>
       <c r="D11" t="s">
         <v>60</v>
@@ -2522,10 +2524,10 @@
         <v>125</v>
       </c>
       <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
         <v>65</v>
-      </c>
-      <c r="C12" t="s">
-        <v>66</v>
       </c>
       <c r="D12" t="s">
         <v>59</v>
@@ -2695,10 +2697,10 @@
         <v>126</v>
       </c>
       <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
         <v>65</v>
-      </c>
-      <c r="C13" t="s">
-        <v>66</v>
       </c>
       <c r="D13" t="s">
         <v>58</v>
@@ -2868,10 +2870,10 @@
         <v>127</v>
       </c>
       <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
         <v>65</v>
-      </c>
-      <c r="C14" t="s">
-        <v>66</v>
       </c>
       <c r="D14" t="s">
         <v>58</v>
@@ -3041,10 +3043,10 @@
         <v>128</v>
       </c>
       <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
         <v>65</v>
-      </c>
-      <c r="C15" t="s">
-        <v>66</v>
       </c>
       <c r="D15" t="s">
         <v>60</v>
@@ -3214,10 +3216,10 @@
         <v>129</v>
       </c>
       <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
         <v>65</v>
-      </c>
-      <c r="C16" t="s">
-        <v>66</v>
       </c>
       <c r="D16" t="s">
         <v>60</v>
@@ -3387,10 +3389,10 @@
         <v>130</v>
       </c>
       <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
         <v>65</v>
-      </c>
-      <c r="C17" t="s">
-        <v>66</v>
       </c>
       <c r="D17" t="s">
         <v>58</v>
@@ -3560,10 +3562,10 @@
         <v>131</v>
       </c>
       <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
         <v>65</v>
-      </c>
-      <c r="C18" t="s">
-        <v>66</v>
       </c>
       <c r="D18" t="s">
         <v>59</v>
@@ -3733,10 +3735,10 @@
         <v>132</v>
       </c>
       <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" t="s">
         <v>65</v>
-      </c>
-      <c r="C19" t="s">
-        <v>66</v>
       </c>
       <c r="D19" t="s">
         <v>60</v>
@@ -3906,10 +3908,10 @@
         <v>133</v>
       </c>
       <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
         <v>65</v>
-      </c>
-      <c r="C20" t="s">
-        <v>66</v>
       </c>
       <c r="D20" t="s">
         <v>60</v>
@@ -4079,10 +4081,10 @@
         <v>134</v>
       </c>
       <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
         <v>65</v>
-      </c>
-      <c r="C21" t="s">
-        <v>66</v>
       </c>
       <c r="D21" t="s">
         <v>60</v>
@@ -4252,10 +4254,10 @@
         <v>139</v>
       </c>
       <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
         <v>65</v>
-      </c>
-      <c r="C22" t="s">
-        <v>66</v>
       </c>
       <c r="D22" t="s">
         <v>59</v>
@@ -4425,10 +4427,10 @@
         <v>140</v>
       </c>
       <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
         <v>65</v>
-      </c>
-      <c r="C23" t="s">
-        <v>66</v>
       </c>
       <c r="D23" t="s">
         <v>60</v>
@@ -4598,10 +4600,10 @@
         <v>141</v>
       </c>
       <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" t="s">
         <v>65</v>
-      </c>
-      <c r="C24" t="s">
-        <v>66</v>
       </c>
       <c r="D24" t="s">
         <v>58</v>
@@ -4771,10 +4773,10 @@
         <v>142</v>
       </c>
       <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
         <v>65</v>
-      </c>
-      <c r="C25" t="s">
-        <v>66</v>
       </c>
       <c r="D25" t="s">
         <v>60</v>
@@ -4944,10 +4946,10 @@
         <v>143</v>
       </c>
       <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" t="s">
         <v>65</v>
-      </c>
-      <c r="C26" t="s">
-        <v>66</v>
       </c>
       <c r="D26" t="s">
         <v>59</v>
@@ -5117,10 +5119,10 @@
         <v>144</v>
       </c>
       <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" t="s">
         <v>65</v>
-      </c>
-      <c r="C27" t="s">
-        <v>66</v>
       </c>
       <c r="D27" t="s">
         <v>60</v>
@@ -5290,10 +5292,10 @@
         <v>145</v>
       </c>
       <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" t="s">
         <v>65</v>
-      </c>
-      <c r="C28" t="s">
-        <v>66</v>
       </c>
       <c r="D28" t="s">
         <v>59</v>
@@ -5463,10 +5465,10 @@
         <v>146</v>
       </c>
       <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" t="s">
         <v>65</v>
-      </c>
-      <c r="C29" t="s">
-        <v>66</v>
       </c>
       <c r="D29" t="s">
         <v>58</v>
@@ -5636,10 +5638,10 @@
         <v>147</v>
       </c>
       <c r="B30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" t="s">
         <v>65</v>
-      </c>
-      <c r="C30" t="s">
-        <v>66</v>
       </c>
       <c r="D30" t="s">
         <v>59</v>
@@ -5809,10 +5811,10 @@
         <v>148</v>
       </c>
       <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
         <v>65</v>
-      </c>
-      <c r="C31" t="s">
-        <v>66</v>
       </c>
       <c r="D31" t="s">
         <v>59</v>
@@ -5982,10 +5984,10 @@
         <v>149</v>
       </c>
       <c r="B32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" t="s">
         <v>65</v>
-      </c>
-      <c r="C32" t="s">
-        <v>66</v>
       </c>
       <c r="D32" t="s">
         <v>58</v>
@@ -6155,10 +6157,10 @@
         <v>150</v>
       </c>
       <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
         <v>65</v>
-      </c>
-      <c r="C33" t="s">
-        <v>66</v>
       </c>
       <c r="D33" t="s">
         <v>58</v>
@@ -6328,10 +6330,10 @@
         <v>151</v>
       </c>
       <c r="B34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" t="s">
         <v>65</v>
-      </c>
-      <c r="C34" t="s">
-        <v>66</v>
       </c>
       <c r="D34" t="s">
         <v>59</v>
@@ -6501,10 +6503,10 @@
         <v>152</v>
       </c>
       <c r="B35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" t="s">
         <v>65</v>
-      </c>
-      <c r="C35" t="s">
-        <v>66</v>
       </c>
       <c r="D35" t="s">
         <v>59</v>
@@ -6674,10 +6676,10 @@
         <v>153</v>
       </c>
       <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" t="s">
         <v>65</v>
-      </c>
-      <c r="C36" t="s">
-        <v>66</v>
       </c>
       <c r="D36" t="s">
         <v>59</v>
@@ -6847,10 +6849,10 @@
         <v>154</v>
       </c>
       <c r="B37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" t="s">
         <v>65</v>
-      </c>
-      <c r="C37" t="s">
-        <v>66</v>
       </c>
       <c r="D37" t="s">
         <v>59</v>
@@ -7020,10 +7022,10 @@
         <v>155</v>
       </c>
       <c r="B38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" t="s">
         <v>65</v>
-      </c>
-      <c r="C38" t="s">
-        <v>66</v>
       </c>
       <c r="D38" t="s">
         <v>59</v>
@@ -7193,10 +7195,10 @@
         <v>156</v>
       </c>
       <c r="B39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" t="s">
         <v>65</v>
-      </c>
-      <c r="C39" t="s">
-        <v>66</v>
       </c>
       <c r="D39" t="s">
         <v>58</v>
@@ -7366,10 +7368,10 @@
         <v>157</v>
       </c>
       <c r="B40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" t="s">
         <v>65</v>
-      </c>
-      <c r="C40" t="s">
-        <v>66</v>
       </c>
       <c r="D40" t="s">
         <v>58</v>
@@ -7539,10 +7541,10 @@
         <v>158</v>
       </c>
       <c r="B41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" t="s">
         <v>65</v>
-      </c>
-      <c r="C41" t="s">
-        <v>66</v>
       </c>
       <c r="D41" t="s">
         <v>58</v>
@@ -7712,10 +7714,10 @@
         <v>159</v>
       </c>
       <c r="B42" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" t="s">
         <v>65</v>
-      </c>
-      <c r="C42" t="s">
-        <v>66</v>
       </c>
       <c r="D42" t="s">
         <v>59</v>
@@ -7885,10 +7887,10 @@
         <v>160</v>
       </c>
       <c r="B43" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" t="s">
         <v>65</v>
-      </c>
-      <c r="C43" t="s">
-        <v>66</v>
       </c>
       <c r="D43" t="s">
         <v>58</v>
@@ -8058,10 +8060,10 @@
         <v>161</v>
       </c>
       <c r="B44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" t="s">
         <v>65</v>
-      </c>
-      <c r="C44" t="s">
-        <v>66</v>
       </c>
       <c r="D44" t="s">
         <v>58</v>
@@ -8231,10 +8233,10 @@
         <v>162</v>
       </c>
       <c r="B45" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" t="s">
         <v>65</v>
-      </c>
-      <c r="C45" t="s">
-        <v>66</v>
       </c>
       <c r="D45" t="s">
         <v>59</v>
@@ -8404,10 +8406,10 @@
         <v>163</v>
       </c>
       <c r="B46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" t="s">
         <v>65</v>
-      </c>
-      <c r="C46" t="s">
-        <v>66</v>
       </c>
       <c r="D46" t="s">
         <v>58</v>
@@ -8577,10 +8579,10 @@
         <v>165</v>
       </c>
       <c r="B47" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" t="s">
         <v>65</v>
-      </c>
-      <c r="C47" t="s">
-        <v>66</v>
       </c>
       <c r="D47" t="s">
         <v>59</v>
@@ -8750,10 +8752,10 @@
         <v>168</v>
       </c>
       <c r="B48" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" t="s">
         <v>65</v>
-      </c>
-      <c r="C48" t="s">
-        <v>66</v>
       </c>
       <c r="D48" t="s">
         <v>60</v>
@@ -8923,10 +8925,10 @@
         <v>169</v>
       </c>
       <c r="B49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" t="s">
         <v>65</v>
-      </c>
-      <c r="C49" t="s">
-        <v>66</v>
       </c>
       <c r="D49" t="s">
         <v>61</v>
@@ -9096,10 +9098,10 @@
         <v>171</v>
       </c>
       <c r="B50" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" t="s">
         <v>65</v>
-      </c>
-      <c r="C50" t="s">
-        <v>66</v>
       </c>
       <c r="D50" t="s">
         <v>59</v>
@@ -9269,10 +9271,10 @@
         <v>179</v>
       </c>
       <c r="B51" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51" t="s">
         <v>65</v>
-      </c>
-      <c r="C51" t="s">
-        <v>66</v>
       </c>
       <c r="D51" t="s">
         <v>61</v>
@@ -9442,10 +9444,10 @@
         <v>180</v>
       </c>
       <c r="B52" t="s">
+        <v>64</v>
+      </c>
+      <c r="C52" t="s">
         <v>65</v>
-      </c>
-      <c r="C52" t="s">
-        <v>66</v>
       </c>
       <c r="D52" t="s">
         <v>61</v>
@@ -9615,10 +9617,10 @@
         <v>181</v>
       </c>
       <c r="B53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" t="s">
         <v>65</v>
-      </c>
-      <c r="C53" t="s">
-        <v>66</v>
       </c>
       <c r="D53" t="s">
         <v>61</v>
@@ -9788,10 +9790,10 @@
         <v>183</v>
       </c>
       <c r="B54" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" t="s">
         <v>65</v>
-      </c>
-      <c r="C54" t="s">
-        <v>66</v>
       </c>
       <c r="D54" t="s">
         <v>59</v>
@@ -9961,10 +9963,10 @@
         <v>191</v>
       </c>
       <c r="B55" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55" t="s">
         <v>65</v>
-      </c>
-      <c r="C55" t="s">
-        <v>66</v>
       </c>
       <c r="D55" t="s">
         <v>60</v>
@@ -10134,10 +10136,10 @@
         <v>192</v>
       </c>
       <c r="B56" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" t="s">
         <v>65</v>
-      </c>
-      <c r="C56" t="s">
-        <v>66</v>
       </c>
       <c r="D56" t="s">
         <v>60</v>
@@ -10307,10 +10309,10 @@
         <v>193</v>
       </c>
       <c r="B57" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" t="s">
         <v>65</v>
-      </c>
-      <c r="C57" t="s">
-        <v>66</v>
       </c>
       <c r="D57" t="s">
         <v>61</v>
@@ -10480,10 +10482,10 @@
         <v>194</v>
       </c>
       <c r="B58" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" t="s">
         <v>65</v>
-      </c>
-      <c r="C58" t="s">
-        <v>66</v>
       </c>
       <c r="D58" t="s">
         <v>58</v>
@@ -10653,10 +10655,10 @@
         <v>659</v>
       </c>
       <c r="B59" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" t="s">
         <v>65</v>
-      </c>
-      <c r="C59" t="s">
-        <v>66</v>
       </c>
       <c r="D59" t="s">
         <v>55</v>
@@ -10826,10 +10828,10 @@
         <v>998</v>
       </c>
       <c r="B60" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" t="s">
         <v>65</v>
-      </c>
-      <c r="C60" t="s">
-        <v>66</v>
       </c>
       <c r="D60" t="s">
         <v>56</v>
@@ -10999,10 +11001,10 @@
         <v>1050</v>
       </c>
       <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" t="s">
         <v>65</v>
-      </c>
-      <c r="C61" t="s">
-        <v>66</v>
       </c>
       <c r="D61" t="s">
         <v>55</v>
@@ -11172,10 +11174,10 @@
         <v>1649</v>
       </c>
       <c r="B62" t="s">
+        <v>64</v>
+      </c>
+      <c r="C62" t="s">
         <v>65</v>
-      </c>
-      <c r="C62" t="s">
-        <v>66</v>
       </c>
       <c r="D62" t="s">
         <v>56</v>
@@ -11345,10 +11347,10 @@
         <v>1650</v>
       </c>
       <c r="B63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" t="s">
         <v>65</v>
-      </c>
-      <c r="C63" t="s">
-        <v>66</v>
       </c>
       <c r="D63" t="s">
         <v>56</v>
@@ -11518,10 +11520,10 @@
         <v>3792</v>
       </c>
       <c r="B64" t="s">
+        <v>64</v>
+      </c>
+      <c r="C64" t="s">
         <v>65</v>
-      </c>
-      <c r="C64" t="s">
-        <v>66</v>
       </c>
       <c r="D64" t="s">
         <v>56</v>
@@ -11691,10 +11693,10 @@
         <v>4468</v>
       </c>
       <c r="B65" t="s">
+        <v>64</v>
+      </c>
+      <c r="C65" t="s">
         <v>65</v>
-      </c>
-      <c r="C65" t="s">
-        <v>66</v>
       </c>
       <c r="D65" t="s">
         <v>56</v>
@@ -11864,10 +11866,10 @@
         <v>4753</v>
       </c>
       <c r="B66" t="s">
+        <v>64</v>
+      </c>
+      <c r="C66" t="s">
         <v>65</v>
-      </c>
-      <c r="C66" t="s">
-        <v>66</v>
       </c>
       <c r="D66" t="s">
         <v>61</v>
@@ -12037,10 +12039,10 @@
         <v>4754</v>
       </c>
       <c r="B67" t="s">
+        <v>64</v>
+      </c>
+      <c r="C67" t="s">
         <v>65</v>
-      </c>
-      <c r="C67" t="s">
-        <v>66</v>
       </c>
       <c r="D67" t="s">
         <v>58</v>
@@ -12210,10 +12212,10 @@
         <v>4762</v>
       </c>
       <c r="B68" t="s">
+        <v>64</v>
+      </c>
+      <c r="C68" t="s">
         <v>65</v>
-      </c>
-      <c r="C68" t="s">
-        <v>66</v>
       </c>
       <c r="D68" t="s">
         <v>58</v>
@@ -12383,10 +12385,10 @@
         <v>4768</v>
       </c>
       <c r="B69" t="s">
+        <v>64</v>
+      </c>
+      <c r="C69" t="s">
         <v>65</v>
-      </c>
-      <c r="C69" t="s">
-        <v>66</v>
       </c>
       <c r="D69" t="s">
         <v>61</v>
@@ -12556,10 +12558,10 @@
         <v>4770</v>
       </c>
       <c r="B70" t="s">
+        <v>64</v>
+      </c>
+      <c r="C70" t="s">
         <v>65</v>
-      </c>
-      <c r="C70" t="s">
-        <v>66</v>
       </c>
       <c r="D70" t="s">
         <v>58</v>
@@ -12729,10 +12731,10 @@
         <v>4772</v>
       </c>
       <c r="B71" t="s">
+        <v>64</v>
+      </c>
+      <c r="C71" t="s">
         <v>65</v>
-      </c>
-      <c r="C71" t="s">
-        <v>66</v>
       </c>
       <c r="D71" t="s">
         <v>58</v>
@@ -12902,10 +12904,10 @@
         <v>4773</v>
       </c>
       <c r="B72" t="s">
+        <v>64</v>
+      </c>
+      <c r="C72" t="s">
         <v>65</v>
-      </c>
-      <c r="C72" t="s">
-        <v>66</v>
       </c>
       <c r="D72" t="s">
         <v>58</v>
@@ -13075,10 +13077,10 @@
         <v>4804</v>
       </c>
       <c r="B73" t="s">
+        <v>64</v>
+      </c>
+      <c r="C73" t="s">
         <v>65</v>
-      </c>
-      <c r="C73" t="s">
-        <v>66</v>
       </c>
       <c r="D73" t="s">
         <v>58</v>
@@ -13248,10 +13250,10 @@
         <v>4806</v>
       </c>
       <c r="B74" t="s">
+        <v>64</v>
+      </c>
+      <c r="C74" t="s">
         <v>65</v>
-      </c>
-      <c r="C74" t="s">
-        <v>66</v>
       </c>
       <c r="D74" t="s">
         <v>62</v>
@@ -13421,10 +13423,10 @@
         <v>4810</v>
       </c>
       <c r="B75" t="s">
+        <v>64</v>
+      </c>
+      <c r="C75" t="s">
         <v>65</v>
-      </c>
-      <c r="C75" t="s">
-        <v>66</v>
       </c>
       <c r="D75" t="s">
         <v>58</v>
@@ -13594,10 +13596,10 @@
         <v>4823</v>
       </c>
       <c r="B76" t="s">
+        <v>64</v>
+      </c>
+      <c r="C76" t="s">
         <v>65</v>
-      </c>
-      <c r="C76" t="s">
-        <v>66</v>
       </c>
       <c r="D76" t="s">
         <v>58</v>
@@ -13767,10 +13769,10 @@
         <v>4828</v>
       </c>
       <c r="B77" t="s">
+        <v>64</v>
+      </c>
+      <c r="C77" t="s">
         <v>65</v>
-      </c>
-      <c r="C77" t="s">
-        <v>66</v>
       </c>
       <c r="D77" t="s">
         <v>62</v>
@@ -13940,10 +13942,10 @@
         <v>4849</v>
       </c>
       <c r="B78" t="s">
+        <v>64</v>
+      </c>
+      <c r="C78" t="s">
         <v>65</v>
-      </c>
-      <c r="C78" t="s">
-        <v>66</v>
       </c>
       <c r="D78" t="s">
         <v>57</v>
@@ -14113,10 +14115,10 @@
         <v>4861</v>
       </c>
       <c r="B79" t="s">
+        <v>64</v>
+      </c>
+      <c r="C79" t="s">
         <v>65</v>
-      </c>
-      <c r="C79" t="s">
-        <v>66</v>
       </c>
       <c r="D79" t="s">
         <v>56</v>
@@ -14286,10 +14288,10 @@
         <v>4875</v>
       </c>
       <c r="B80" t="s">
+        <v>64</v>
+      </c>
+      <c r="C80" t="s">
         <v>65</v>
-      </c>
-      <c r="C80" t="s">
-        <v>66</v>
       </c>
       <c r="D80" t="s">
         <v>62</v>
@@ -14459,10 +14461,10 @@
         <v>4877</v>
       </c>
       <c r="B81" t="s">
+        <v>64</v>
+      </c>
+      <c r="C81" t="s">
         <v>65</v>
-      </c>
-      <c r="C81" t="s">
-        <v>66</v>
       </c>
       <c r="D81" t="s">
         <v>62</v>
@@ -14632,10 +14634,10 @@
         <v>5156</v>
       </c>
       <c r="B82" t="s">
+        <v>64</v>
+      </c>
+      <c r="C82" t="s">
         <v>65</v>
-      </c>
-      <c r="C82" t="s">
-        <v>66</v>
       </c>
       <c r="D82" t="s">
         <v>56</v>
@@ -14805,10 +14807,10 @@
         <v>5450</v>
       </c>
       <c r="B83" t="s">
+        <v>64</v>
+      </c>
+      <c r="C83" t="s">
         <v>65</v>
-      </c>
-      <c r="C83" t="s">
-        <v>66</v>
       </c>
       <c r="D83" t="s">
         <v>56</v>

</xml_diff>